<commit_message>
Enhance ExcelHandler to update summary formulas dynamically based on new data row count and improve file filtering in VacationProcessor to ignore temporary Excel files. Update global report template.
</commit_message>
<xml_diff>
--- a/templates/global_report_template v3.2.xlsx
+++ b/templates/global_report_template v3.2.xlsx
@@ -13,7 +13,7 @@
   </bookViews>
   <sheets>
     <sheet name="Report" sheetId="1" r:id="rId1"/>
-    <sheet name="rules" sheetId="2" r:id="rId2"/>
+    <sheet name="rules" sheetId="2" state="hidden" r:id="rId2"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Report!$A$8:$K$8</definedName>
@@ -526,6 +526,38 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="9" fontId="1" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="13" xfId="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="9" fontId="4" fillId="6" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="4" fillId="6" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="4" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="3" borderId="9" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -559,13 +591,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="5" borderId="4" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyProtection="1">
-      <protection locked="0"/>
-    </xf>
     <xf numFmtId="0" fontId="7" fillId="5" borderId="5" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
       <protection locked="0"/>
@@ -576,31 +601,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyProtection="1">
       <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="9" fontId="1" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="13" xfId="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="9" fontId="4" fillId="6" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="4" fillId="6" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -887,84 +887,84 @@
   <dimension ref="A1:K11"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection sqref="A1:D1"/>
+      <selection activeCell="B18" sqref="B18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="20.100000000000001" customHeight="1" outlineLevelCol="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="10.7109375" style="3" customWidth="1"/>
     <col min="2" max="2" width="30.7109375" style="3" customWidth="1"/>
-    <col min="3" max="10" width="11.7109375" style="3" customWidth="1" outlineLevel="1"/>
-    <col min="11" max="11" width="30.7109375" style="3" customWidth="1" outlineLevel="1"/>
+    <col min="3" max="10" width="11.7109375" style="3" customWidth="1"/>
+    <col min="11" max="11" width="30.7109375" style="3" customWidth="1"/>
     <col min="12" max="12" width="8.85546875" style="3" customWidth="1"/>
     <col min="13" max="16384" width="8.85546875" style="3"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="21" t="s">
+      <c r="A1" s="31" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="22"/>
-      <c r="C1" s="22"/>
-      <c r="D1" s="23"/>
+      <c r="B1" s="32"/>
+      <c r="C1" s="32"/>
+      <c r="D1" s="33"/>
       <c r="E1" s="17"/>
       <c r="J1" s="4"/>
     </row>
     <row r="2" spans="1:11" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="24" t="s">
+      <c r="A2" s="34" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="25"/>
-      <c r="C2" s="28" t="s">
+      <c r="B2" s="35"/>
+      <c r="C2" s="38" t="s">
         <v>2</v>
       </c>
-      <c r="D2" s="29"/>
+      <c r="D2" s="39"/>
       <c r="E2" s="18"/>
       <c r="J2" s="5"/>
     </row>
     <row r="3" spans="1:11" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="32" t="s">
+      <c r="A3" s="29" t="s">
         <v>3</v>
       </c>
-      <c r="B3" s="33"/>
-      <c r="C3" s="34" t="s">
+      <c r="B3" s="30"/>
+      <c r="C3" s="42" t="s">
         <v>4</v>
       </c>
-      <c r="D3" s="31"/>
+      <c r="D3" s="41"/>
       <c r="E3" s="18"/>
       <c r="J3" s="6"/>
     </row>
     <row r="4" spans="1:11" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="32" t="s">
+      <c r="A4" s="29" t="s">
         <v>5</v>
       </c>
-      <c r="B4" s="33"/>
-      <c r="C4" s="30">
+      <c r="B4" s="30"/>
+      <c r="C4" s="40">
         <v>5</v>
       </c>
-      <c r="D4" s="31"/>
+      <c r="D4" s="41"/>
       <c r="E4" s="18"/>
     </row>
     <row r="5" spans="1:11" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="32" t="s">
+      <c r="A5" s="29" t="s">
         <v>6</v>
       </c>
-      <c r="B5" s="33"/>
-      <c r="C5" s="30">
+      <c r="B5" s="30"/>
+      <c r="C5" s="40">
         <v>8</v>
       </c>
-      <c r="D5" s="31"/>
+      <c r="D5" s="41"/>
       <c r="E5" s="18"/>
     </row>
     <row r="6" spans="1:11" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="35" t="s">
+      <c r="A6" s="43" t="s">
         <v>7</v>
       </c>
-      <c r="B6" s="36"/>
-      <c r="C6" s="26">
+      <c r="B6" s="44"/>
+      <c r="C6" s="36">
         <v>0</v>
       </c>
-      <c r="D6" s="27"/>
+      <c r="D6" s="37"/>
       <c r="E6" s="18"/>
       <c r="F6" s="7"/>
       <c r="G6" s="7"/>
@@ -993,22 +993,22 @@
       <c r="B8" s="12" t="s">
         <v>9</v>
       </c>
-      <c r="C8" s="37" t="s">
+      <c r="C8" s="27" t="s">
         <v>10</v>
       </c>
-      <c r="D8" s="38"/>
-      <c r="E8" s="37" t="s">
+      <c r="D8" s="28"/>
+      <c r="E8" s="27" t="s">
         <v>11</v>
       </c>
-      <c r="F8" s="38"/>
-      <c r="G8" s="37" t="s">
+      <c r="F8" s="28"/>
+      <c r="G8" s="27" t="s">
         <v>12</v>
       </c>
-      <c r="H8" s="38"/>
-      <c r="I8" s="37" t="s">
+      <c r="H8" s="28"/>
+      <c r="I8" s="27" t="s">
         <v>13</v>
       </c>
-      <c r="J8" s="38"/>
+      <c r="J8" s="28"/>
       <c r="K8" s="1" t="s">
         <v>14</v>
       </c>
@@ -1020,28 +1020,28 @@
       <c r="B9" s="20" t="s">
         <v>52</v>
       </c>
-      <c r="C9" s="39">
+      <c r="C9" s="21">
         <v>0.5</v>
       </c>
-      <c r="D9" s="40">
+      <c r="D9" s="22">
         <v>4</v>
       </c>
-      <c r="E9" s="39">
+      <c r="E9" s="21">
         <v>0.25</v>
       </c>
-      <c r="F9" s="41">
+      <c r="F9" s="23">
         <v>1</v>
       </c>
-      <c r="G9" s="39">
+      <c r="G9" s="21">
         <v>0.75</v>
       </c>
-      <c r="H9" s="40">
+      <c r="H9" s="22">
         <v>3</v>
       </c>
-      <c r="I9" s="39">
+      <c r="I9" s="21">
         <v>0.25</v>
       </c>
-      <c r="J9" s="42">
+      <c r="J9" s="24">
         <v>1</v>
       </c>
       <c r="K9" s="14" t="s">
@@ -1051,35 +1051,35 @@
     <row r="10" spans="1:11" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="15"/>
       <c r="B10" s="16"/>
-      <c r="C10" s="43">
+      <c r="C10" s="25">
         <f>AVERAGE(C9:C9)</f>
         <v>0.5</v>
       </c>
-      <c r="D10" s="44">
+      <c r="D10" s="26">
         <f>SUM(D9:D9)</f>
         <v>4</v>
       </c>
-      <c r="E10" s="43">
+      <c r="E10" s="25">
         <f>AVERAGE(E9:E9)</f>
         <v>0.25</v>
       </c>
-      <c r="F10" s="44">
+      <c r="F10" s="26">
         <f>SUM(F9:F9)</f>
         <v>1</v>
       </c>
-      <c r="G10" s="43">
+      <c r="G10" s="25">
         <f>AVERAGE(G9:G9)</f>
         <v>0.75</v>
       </c>
-      <c r="H10" s="44">
+      <c r="H10" s="26">
         <f>SUM(H9:H9)</f>
         <v>3</v>
       </c>
-      <c r="I10" s="43">
+      <c r="I10" s="25">
         <f>AVERAGE(I9:I9)</f>
         <v>0.25</v>
       </c>
-      <c r="J10" s="44">
+      <c r="J10" s="26">
         <f>SUM(J9:J9)</f>
         <v>1</v>
       </c>
@@ -1091,11 +1091,6 @@
   </sheetData>
   <autoFilter ref="A8:K8"/>
   <mergeCells count="15">
-    <mergeCell ref="E8:F8"/>
-    <mergeCell ref="G8:H8"/>
-    <mergeCell ref="I8:J8"/>
-    <mergeCell ref="C8:D8"/>
-    <mergeCell ref="A4:B4"/>
     <mergeCell ref="A1:D1"/>
     <mergeCell ref="A2:B2"/>
     <mergeCell ref="C6:D6"/>
@@ -1106,6 +1101,11 @@
     <mergeCell ref="A3:B3"/>
     <mergeCell ref="A6:B6"/>
     <mergeCell ref="C4:D4"/>
+    <mergeCell ref="E8:F8"/>
+    <mergeCell ref="G8:H8"/>
+    <mergeCell ref="I8:J8"/>
+    <mergeCell ref="C8:D8"/>
+    <mergeCell ref="A4:B4"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>